<commit_message>
Add support for header bidding
</commit_message>
<xml_diff>
--- a/src/test/resources/input_files/HBInput.xlsx
+++ b/src/test/resources/input_files/HBInput.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="39">
   <si>
     <t>Test Scenario</t>
   </si>
@@ -46,22 +46,6 @@
   </si>
   <si>
     <t>RESPONSE</t>
-  </si>
-  <si>
-    <t>{"x-ut-hb-params":[ 
- {
- "bidRequestId": "21b46f0d859b33",
- "domain": "cnn.com",
- "placementId": 10433394,
- "publisherId": 12345,
- "sizes": [
- [300, 250],
- [300, 600]
- ],
- "timeout": 700,
- "hbadaptor": "prebid",
- "params": {}
-}]}</t>
   </si>
   <si>
     <t>[{
@@ -179,11 +163,55 @@
     <t>{"experiment":null,"eligibleAds":[]}</t>
   </si>
   <si>
+    <t>send HB request without params</t>
+  </si>
+  <si>
+    <t>Send HB basic request</t>
+  </si>
+  <si>
+    <t>Optimize</t>
+  </si>
+  <si>
+    <t>Send HB request to optimizer</t>
+  </si>
+  <si>
+    <t>Send HB request with Empty domain</t>
+  </si>
+  <si>
+    <t>Send HB request with Empty placementID</t>
+  </si>
+  <si>
+    <t>StatusCode</t>
+  </si>
+  <si>
+    <t>Ranker.com</t>
+  </si>
+  <si>
+    <t>stgads.undertone.com</t>
+  </si>
+  <si>
     <t>{"x-ut-hb-params":[ 
  {
  "bidRequestId": "21b46f0d859b33",
- "domain": "cnn.com",
+ "domain": "Ranker.com",
  "placementId": 10433394,
+ "publisherId": 3470,
+ "sizes": [
+ [300, 250],
+ [300, 600]
+ ],
+ "timeout": 700,
+ "hbadaptor": "prebid",
+ "params": {}
+}]}</t>
+  </si>
+  <si>
+    <t>{"x-ut-hb-params":[ 
+ {
+ "bidRequestId": "21b46f0d859b33",
+ "domain": "Ranker.com",
+ "placementId": 10433394,
+ "publisherId": 3470,
  "sizes": [
  [300, 250],
  [300, 600]
@@ -191,30 +219,16 @@
  "timeout": 700,
  "hbadaptor": "prebid",
  "params": {"placementId" : "10433394",
-                        "publisherId" : 12345
+                        "publisherId" : 3470
 }
 }]}</t>
-  </si>
-  <si>
-    <t>send HB request without params</t>
-  </si>
-  <si>
-    <t>Send HB basic request</t>
-  </si>
-  <si>
-    <t>Optimize</t>
-  </si>
-  <si>
-    <t>Send HB request to optimizer</t>
-  </si>
-  <si>
-    <t>Send HB request with Empty domain</t>
   </si>
   <si>
     <t>{"x-ut-hb-params":[ 
  {
  "bidRequestId": "21b46f0d859b33",
  "placementId": 10433394,
+ "publisherId": 3470,
  "sizes": [
  [300, 250],
  [300, 600]
@@ -222,36 +236,82 @@
  "timeout": 700,
  "hbadaptor": "prebid",
  "params": {"placementId" : "10433394",
-                        "publisherId" : 12345
+                        "publisherId" : 3470
 }
 }]}</t>
-  </si>
-  <si>
-    <t>Send HB request with Empty placementID</t>
   </si>
   <si>
     <t>{"x-ut-hb-params":[ 
  {
  "bidRequestId": "21b46f0d859b33",
+ "domain": "Ranker.com",
+ "publisherId": 3470,
  "sizes": [
  [300, 250],
  [300, 600]
  ],
  "timeout": 700,
  "hbadaptor": "prebid",
- "params": {
-                        "publisherId" : 12345
+ "params": {"publisherId" : 3470
 }
 }]}</t>
   </si>
   <si>
-    <t>StatusCode</t>
-  </si>
-  <si>
-    <t>Ranker.com</t>
-  </si>
-  <si>
-    <t>stgads.undertone.com</t>
+    <t>Send HB request with Empty sizes</t>
+  </si>
+  <si>
+    <t>Send HB request with Empty timeout</t>
+  </si>
+  <si>
+    <t>{"x-ut-hb-params":[ 
+ {
+ "bidRequestId": "21b46f0d859b33",
+ "domain": "Ranker.com",
+ "placementId": 10433394,
+ "publisherId": 3470,
+ "sizes": [],
+ "timeout": 700,
+ "hbadaptor": "prebid",
+ "params": {"placementId" : "10433394",
+                        "publisherId" : 3470
+}
+}]}</t>
+  </si>
+  <si>
+    <t>{"x-ut-hb-params":[ 
+ {
+ "bidRequestId": "21b46f0d859b33",
+ "domain": "Ranker.com",
+ "placementId": 10433394,
+ "publisherId": 3470,
+ "sizes": [
+ [300, 250],
+ [300, 600]
+ ],
+ "timeout": ,
+ "hbadaptor": "prebid",
+ "params": {"placementId" : "10433394",
+                        "publisherId" : 3470
+}
+}]}</t>
+  </si>
+  <si>
+    <t>Send HB request with wrong values</t>
+  </si>
+  <si>
+    <t>{"x-ut-hb-params":[ 
+ {
+ "bidRequestId": "21b46f0d859b33",
+ "domain": "Ranker.com",
+ "placementId": 10433394,
+ "publisherId": 0000,
+ "sizes": [],
+ "timeout": 700,
+ "hbadaptor": "prebida",
+ "params": {"placementId" : "10433394",
+                        "publisherId" : 0000
+}
+}]}</t>
   </si>
 </sst>
 </file>
@@ -659,8 +719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{605AD3CC-41F2-49AA-9F70-5058AA94EA10}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -697,39 +757,39 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="405" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C2" s="5">
         <v>3470</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>7</v>
       </c>
       <c r="G2" s="3">
         <v>0</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I2" s="2">
         <v>200</v>
@@ -737,138 +797,219 @@
     </row>
     <row r="3" spans="1:9" ht="405" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C3" s="5">
         <v>3470</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G3" s="3">
         <v>0</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I3" s="2">
         <v>204</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="256.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="270.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C4" s="10">
         <v>3470</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3">
         <v>0</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I4" s="2">
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="256.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="270.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C5" s="10">
         <v>3470</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3">
         <v>1</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I5" s="2">
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="242.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="256.5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C6" s="10">
         <v>3470</v>
       </c>
       <c r="D6" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3">
         <v>0</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I6" s="2">
         <v>204</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="213.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="228" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="9" t="s">
         <v>28</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>32</v>
       </c>
       <c r="C7" s="10">
         <v>3470</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3">
         <v>0</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I7" s="2">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="8" customFormat="1" ht="228" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="10">
+        <v>3470</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3">
+        <v>0</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" s="8">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="8" customFormat="1" ht="270.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="10">
+        <v>3470</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3">
+        <v>0</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" s="8">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="8" customFormat="1" ht="228" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="10">
+        <v>3470</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3">
+        <v>0</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" s="8">
         <v>204</v>
       </c>
     </row>
@@ -920,56 +1061,56 @@
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G1" s="3">
         <v>0</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="G2" s="2">
         <v>0</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="2" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>17</v>
       </c>
       <c r="G3" s="2">
         <v>0</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change Ranker to ranker
</commit_message>
<xml_diff>
--- a/src/test/resources/input_files/HBInput.xlsx
+++ b/src/test/resources/input_files/HBInput.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="70">
   <si>
     <t>Test Scenario</t>
   </si>
@@ -370,13 +370,21 @@
     <t>send Ranker HB request without params</t>
   </si>
   <si>
-    <t>Ranker.com</t>
+    <t>send Ranker HB request without publlisherID configured</t>
+  </si>
+  <si>
+    <t>Send Ranker HB basic request</t>
+  </si>
+  <si>
+    <t>Send Ranker HB request to optimizer</t>
+  </si>
+  <si>
+    <t>Send Ranker HB request with Empty domain</t>
   </si>
   <si>
     <t>{"x-ut-hb-params":[ 
  {
  "bidRequestId": "21b46f0d859b33",
- "domain": "Ranker.com",
  "placementId": "10433394",
  "publisherId": 3470,
  "sizes": [
@@ -385,35 +393,37 @@
  ],
  "timeout": 700,
  "hbadaptor": "prebid",
- "params": {}
-}]}</t>
-  </si>
-  <si>
-    <t>send Ranker HB request without publlisherID configured</t>
+ "params": {"placementId" : "10433394",
+                        "publisherId" : 3470
+}
+}]}</t>
+  </si>
+  <si>
+    <t>Send Ranker HB request with Empty placementID</t>
+  </si>
+  <si>
+    <t>Send Ranker HB request with Empty sizes</t>
+  </si>
+  <si>
+    <t>Send Ranker HB request with Empty timeout</t>
+  </si>
+  <si>
+    <t>Send Ranker HB request with wrong values</t>
+  </si>
+  <si>
+    <t>Send Ranker HB request with no 1X1 size</t>
+  </si>
+  <si>
+    <t>Send Ranker HB request with one size</t>
+  </si>
+  <si>
+    <t>ranker.com</t>
   </si>
   <si>
     <t>{"x-ut-hb-params":[ 
  {
  "bidRequestId": "21b46f0d859b33",
- "domain": "Ranker.com",
- "placementId": "10433394",
- "sizes": [
- [1, 1],
- [160, 600]
- ],
- "timeout": 700,
- "hbadaptor": "prebid",
- "params": {}
-}]}</t>
-  </si>
-  <si>
-    <t>Send Ranker HB basic request</t>
-  </si>
-  <si>
-    <t>{"x-ut-hb-params":[ 
- {
- "bidRequestId": "21b46f0d859b33",
- "domain": "Ranker.com",
+ "domain": "ranker.com",
  "placementId": "10433394",
  "publisherId": 3470,
  "sizes": [
@@ -422,19 +432,29 @@
  ],
  "timeout": 700,
  "hbadaptor": "prebid",
- "params": {"placementId" : "10433394",
-                        "publisherId" : 3470
-}
-}]}</t>
-  </si>
-  <si>
-    <t>Send Ranker HB request to optimizer</t>
-  </si>
-  <si>
-    <t>{"x-ut-hb-params":[ 
- {
- "bidRequestId": "21b46f0d859b99",
- "domain": "Ranker.com",
+ "params": {}
+}]}</t>
+  </si>
+  <si>
+    <t>{"x-ut-hb-params":[ 
+ {
+ "bidRequestId": "21b46f0d859b33",
+ "domain": "ranker.com",
+ "placementId": "10433394",
+ "sizes": [
+ [1, 1],
+ [160, 600]
+ ],
+ "timeout": 700,
+ "hbadaptor": "prebid",
+ "params": {}
+}]}</t>
+  </si>
+  <si>
+    <t>{"x-ut-hb-params":[ 
+ {
+ "bidRequestId": "21b46f0d859b33",
+ "domain": "ranker.com",
  "placementId": "10433394",
  "publisherId": 3470,
  "sizes": [
@@ -449,12 +469,10 @@
 }]}</t>
   </si>
   <si>
-    <t>Send Ranker HB request with Empty domain</t>
-  </si>
-  <si>
-    <t>{"x-ut-hb-params":[ 
- {
- "bidRequestId": "21b46f0d859b33",
+    <t>{"x-ut-hb-params":[ 
+ {
+ "bidRequestId": "21b46f0d859b99",
+ "domain": "ranker.com",
  "placementId": "10433394",
  "publisherId": 3470,
  "sizes": [
@@ -469,13 +487,10 @@
 }]}</t>
   </si>
   <si>
-    <t>Send Ranker HB request with Empty placementID</t>
-  </si>
-  <si>
     <t>{"x-ut-hb-params":[ 
  {
  "bidRequestId": "21b46f0d859b33",
- "domain": "Ranker.com",
+ "domain": "ranker.com",
  "publisherId":3470,
  "sizes": [
  [1, 1],
@@ -488,13 +503,10 @@
 }]}</t>
   </si>
   <si>
-    <t>Send Ranker HB request with Empty sizes</t>
-  </si>
-  <si>
     <t>{"x-ut-hb-params":[ 
  {
  "bidRequestId": "21b46f0d859b33",
- "domain": "Ranker.com",
+ "domain": "ranker.com",
  "placementId": "10433394",
  "publisherId": 3470,
  "sizes": [],
@@ -506,13 +518,10 @@
 }]}</t>
   </si>
   <si>
-    <t>Send Ranker HB request with Empty timeout</t>
-  </si>
-  <si>
     <t>{"x-ut-hb-params":[ 
  {
  "bidRequestId": "21b46f0d859b33",
- "domain": "Ranker.com",
+ "domain": "ranker.com",
  "placementId": "10433394",
  "publisherId": 3470,
  "sizes": [
@@ -526,13 +535,25 @@
 }]}</t>
   </si>
   <si>
-    <t>Send Ranker HB request with wrong values</t>
+    <t>{"x-ut-hb-params":[ 
+ {
+ "bidRequestId": "21b46f0d859b33",
+ "domain": "ranker.com",
+ "placementId": "10433394",
+ "publisherId": 0000,
+ "sizes": [],
+ "timeout": 700,
+ "hbadaptor": "prebida",
+ "params": {"placementId" : "10433394",
+                        "publisherId" : 0000
+}
+}]}</t>
   </si>
   <si>
     <t>{"x-ut-hb-params":[ 
  {
  "bidRequestId": "21b46f0d859b47",
- "domain": "Ranker.com",
+ "domain": "ranker.com",
  "placementId": "10433394",
  "publisherId": 3470,
  "sizes": [
@@ -546,13 +567,10 @@
 }]}</t>
   </si>
   <si>
-    <t>Send Ranker HB request with no 1X1 size</t>
-  </si>
-  <si>
     <t>{"x-ut-hb-params":[ 
  {
  "bidRequestId": "21b46f0d859b47",
- "domain": "Ranker.com",
+ "domain": "ranker.com",
  "placementId": "10433394",
  "publisherId": 3470,
  "sizes": [
@@ -564,9 +582,6 @@
                         "publisherId" : 3470
 }
 }]}</t>
-  </si>
-  <si>
-    <t>Send Ranker HB request with one size</t>
   </si>
 </sst>
 </file>
@@ -971,7 +986,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{605AD3CC-41F2-49AA-9F70-5058AA94EA10}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
@@ -1336,10 +1351,10 @@
         <v>3470</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>42</v>
@@ -1356,7 +1371,7 @@
     </row>
     <row r="14" spans="1:9" s="7" customFormat="1" ht="213.75" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>29</v>
@@ -1365,10 +1380,10 @@
         <v>3470</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3">
@@ -1383,7 +1398,7 @@
     </row>
     <row r="15" spans="1:9" s="7" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>29</v>
@@ -1392,10 +1407,10 @@
         <v>3470</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>42</v>
@@ -1412,7 +1427,7 @@
     </row>
     <row r="16" spans="1:9" s="7" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>29</v>
@@ -1421,10 +1436,10 @@
         <v>3470</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>43</v>
@@ -1441,7 +1456,7 @@
     </row>
     <row r="17" spans="1:9" s="7" customFormat="1" ht="270.75" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>29</v>
@@ -1450,10 +1465,10 @@
         <v>3470</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3">
@@ -1468,7 +1483,7 @@
     </row>
     <row r="18" spans="1:9" s="7" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>29</v>
@@ -1477,10 +1492,10 @@
         <v>3470</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>44</v>
@@ -1497,7 +1512,7 @@
     </row>
     <row r="19" spans="1:9" s="7" customFormat="1" ht="242.25" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>29</v>
@@ -1506,10 +1521,10 @@
         <v>3470</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3">
@@ -1524,7 +1539,7 @@
     </row>
     <row r="20" spans="1:9" s="7" customFormat="1" ht="270.75" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>29</v>
@@ -1533,10 +1548,10 @@
         <v>3470</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3">
@@ -1549,9 +1564,9 @@
         <v>204</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="7" customFormat="1" ht="270.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" s="7" customFormat="1" ht="242.25" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>29</v>
@@ -1560,10 +1575,10 @@
         <v>3673</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3">
@@ -1578,7 +1593,7 @@
     </row>
     <row r="22" spans="1:9" s="7" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>29</v>
@@ -1587,10 +1602,10 @@
         <v>3470</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>46</v>
@@ -1607,7 +1622,7 @@
     </row>
     <row r="23" spans="1:9" s="7" customFormat="1" ht="270.75" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>29</v>
@@ -1616,10 +1631,10 @@
         <v>3470</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3">

</xml_diff>

<commit_message>
change Ranker to ranker 2
</commit_message>
<xml_diff>
--- a/src/test/resources/input_files/HBInput.xlsx
+++ b/src/test/resources/input_files/HBInput.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="70">
   <si>
     <t>Test Scenario</t>
   </si>
@@ -370,13 +370,21 @@
     <t>send Ranker HB request without params</t>
   </si>
   <si>
-    <t>Ranker.com</t>
+    <t>send Ranker HB request without publlisherID configured</t>
+  </si>
+  <si>
+    <t>Send Ranker HB basic request</t>
+  </si>
+  <si>
+    <t>Send Ranker HB request to optimizer</t>
+  </si>
+  <si>
+    <t>Send Ranker HB request with Empty domain</t>
   </si>
   <si>
     <t>{"x-ut-hb-params":[ 
  {
  "bidRequestId": "21b46f0d859b33",
- "domain": "Ranker.com",
  "placementId": "10433394",
  "publisherId": 3470,
  "sizes": [
@@ -385,35 +393,37 @@
  ],
  "timeout": 700,
  "hbadaptor": "prebid",
- "params": {}
-}]}</t>
-  </si>
-  <si>
-    <t>send Ranker HB request without publlisherID configured</t>
+ "params": {"placementId" : "10433394",
+                        "publisherId" : 3470
+}
+}]}</t>
+  </si>
+  <si>
+    <t>Send Ranker HB request with Empty placementID</t>
+  </si>
+  <si>
+    <t>Send Ranker HB request with Empty sizes</t>
+  </si>
+  <si>
+    <t>Send Ranker HB request with Empty timeout</t>
+  </si>
+  <si>
+    <t>Send Ranker HB request with wrong values</t>
+  </si>
+  <si>
+    <t>Send Ranker HB request with no 1X1 size</t>
+  </si>
+  <si>
+    <t>Send Ranker HB request with one size</t>
+  </si>
+  <si>
+    <t>ranker.com</t>
   </si>
   <si>
     <t>{"x-ut-hb-params":[ 
  {
  "bidRequestId": "21b46f0d859b33",
- "domain": "Ranker.com",
- "placementId": "10433394",
- "sizes": [
- [1, 1],
- [160, 600]
- ],
- "timeout": 700,
- "hbadaptor": "prebid",
- "params": {}
-}]}</t>
-  </si>
-  <si>
-    <t>Send Ranker HB basic request</t>
-  </si>
-  <si>
-    <t>{"x-ut-hb-params":[ 
- {
- "bidRequestId": "21b46f0d859b33",
- "domain": "Ranker.com",
+ "domain": "ranker.com",
  "placementId": "10433394",
  "publisherId": 3470,
  "sizes": [
@@ -422,19 +432,29 @@
  ],
  "timeout": 700,
  "hbadaptor": "prebid",
- "params": {"placementId" : "10433394",
-                        "publisherId" : 3470
-}
-}]}</t>
-  </si>
-  <si>
-    <t>Send Ranker HB request to optimizer</t>
-  </si>
-  <si>
-    <t>{"x-ut-hb-params":[ 
- {
- "bidRequestId": "21b46f0d859b99",
- "domain": "Ranker.com",
+ "params": {}
+}]}</t>
+  </si>
+  <si>
+    <t>{"x-ut-hb-params":[ 
+ {
+ "bidRequestId": "21b46f0d859b33",
+ "domain": "ranker.com",
+ "placementId": "10433394",
+ "sizes": [
+ [1, 1],
+ [160, 600]
+ ],
+ "timeout": 700,
+ "hbadaptor": "prebid",
+ "params": {}
+}]}</t>
+  </si>
+  <si>
+    <t>{"x-ut-hb-params":[ 
+ {
+ "bidRequestId": "21b46f0d859b33",
+ "domain": "ranker.com",
  "placementId": "10433394",
  "publisherId": 3470,
  "sizes": [
@@ -449,12 +469,10 @@
 }]}</t>
   </si>
   <si>
-    <t>Send Ranker HB request with Empty domain</t>
-  </si>
-  <si>
-    <t>{"x-ut-hb-params":[ 
- {
- "bidRequestId": "21b46f0d859b33",
+    <t>{"x-ut-hb-params":[ 
+ {
+ "bidRequestId": "21b46f0d859b99",
+ "domain": "ranker.com",
  "placementId": "10433394",
  "publisherId": 3470,
  "sizes": [
@@ -469,13 +487,10 @@
 }]}</t>
   </si>
   <si>
-    <t>Send Ranker HB request with Empty placementID</t>
-  </si>
-  <si>
     <t>{"x-ut-hb-params":[ 
  {
  "bidRequestId": "21b46f0d859b33",
- "domain": "Ranker.com",
+ "domain": "ranker.com",
  "publisherId":3470,
  "sizes": [
  [1, 1],
@@ -488,13 +503,10 @@
 }]}</t>
   </si>
   <si>
-    <t>Send Ranker HB request with Empty sizes</t>
-  </si>
-  <si>
     <t>{"x-ut-hb-params":[ 
  {
  "bidRequestId": "21b46f0d859b33",
- "domain": "Ranker.com",
+ "domain": "ranker.com",
  "placementId": "10433394",
  "publisherId": 3470,
  "sizes": [],
@@ -506,13 +518,10 @@
 }]}</t>
   </si>
   <si>
-    <t>Send Ranker HB request with Empty timeout</t>
-  </si>
-  <si>
     <t>{"x-ut-hb-params":[ 
  {
  "bidRequestId": "21b46f0d859b33",
- "domain": "Ranker.com",
+ "domain": "ranker.com",
  "placementId": "10433394",
  "publisherId": 3470,
  "sizes": [
@@ -526,13 +535,25 @@
 }]}</t>
   </si>
   <si>
-    <t>Send Ranker HB request with wrong values</t>
+    <t>{"x-ut-hb-params":[ 
+ {
+ "bidRequestId": "21b46f0d859b33",
+ "domain": "ranker.com",
+ "placementId": "10433394",
+ "publisherId": 0000,
+ "sizes": [],
+ "timeout": 700,
+ "hbadaptor": "prebida",
+ "params": {"placementId" : "10433394",
+                        "publisherId" : 0000
+}
+}]}</t>
   </si>
   <si>
     <t>{"x-ut-hb-params":[ 
  {
  "bidRequestId": "21b46f0d859b47",
- "domain": "Ranker.com",
+ "domain": "ranker.com",
  "placementId": "10433394",
  "publisherId": 3470,
  "sizes": [
@@ -546,13 +567,10 @@
 }]}</t>
   </si>
   <si>
-    <t>Send Ranker HB request with no 1X1 size</t>
-  </si>
-  <si>
     <t>{"x-ut-hb-params":[ 
  {
  "bidRequestId": "21b46f0d859b47",
- "domain": "Ranker.com",
+ "domain": "ranker.com",
  "placementId": "10433394",
  "publisherId": 3470,
  "sizes": [
@@ -564,9 +582,6 @@
                         "publisherId" : 3470
 }
 }]}</t>
-  </si>
-  <si>
-    <t>Send Ranker HB request with one size</t>
   </si>
 </sst>
 </file>
@@ -971,8 +986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{605AD3CC-41F2-49AA-9F70-5058AA94EA10}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1336,10 +1351,10 @@
         <v>3470</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>42</v>
@@ -1356,7 +1371,7 @@
     </row>
     <row r="14" spans="1:9" s="7" customFormat="1" ht="213.75" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>29</v>
@@ -1365,10 +1380,10 @@
         <v>3470</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3">
@@ -1383,7 +1398,7 @@
     </row>
     <row r="15" spans="1:9" s="7" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>29</v>
@@ -1392,10 +1407,10 @@
         <v>3470</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>42</v>
@@ -1412,7 +1427,7 @@
     </row>
     <row r="16" spans="1:9" s="7" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>29</v>
@@ -1421,10 +1436,10 @@
         <v>3470</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>43</v>
@@ -1441,7 +1456,7 @@
     </row>
     <row r="17" spans="1:9" s="7" customFormat="1" ht="270.75" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>29</v>
@@ -1450,10 +1465,10 @@
         <v>3470</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3">
@@ -1468,7 +1483,7 @@
     </row>
     <row r="18" spans="1:9" s="7" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>29</v>
@@ -1477,10 +1492,10 @@
         <v>3470</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>44</v>
@@ -1497,7 +1512,7 @@
     </row>
     <row r="19" spans="1:9" s="7" customFormat="1" ht="242.25" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>29</v>
@@ -1506,10 +1521,10 @@
         <v>3470</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3">
@@ -1524,7 +1539,7 @@
     </row>
     <row r="20" spans="1:9" s="7" customFormat="1" ht="270.75" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>29</v>
@@ -1533,10 +1548,10 @@
         <v>3470</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3">
@@ -1549,9 +1564,9 @@
         <v>204</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="7" customFormat="1" ht="270.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" s="7" customFormat="1" ht="242.25" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>29</v>
@@ -1560,10 +1575,10 @@
         <v>3673</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3">
@@ -1578,7 +1593,7 @@
     </row>
     <row r="22" spans="1:9" s="7" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>29</v>
@@ -1587,10 +1602,10 @@
         <v>3470</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>46</v>
@@ -1607,7 +1622,7 @@
     </row>
     <row r="23" spans="1:9" s="7" customFormat="1" ht="270.75" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>29</v>
@@ -1616,10 +1631,10 @@
         <v>3470</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3">

</xml_diff>

<commit_message>
change Expected results for ranker
</commit_message>
<xml_diff>
--- a/src/test/resources/input_files/HBInput.xlsx
+++ b/src/test/resources/input_files/HBInput.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="74">
   <si>
     <t>Test Scenario</t>
   </si>
@@ -582,6 +582,18 @@
                         "publisherId" : 3470
 }
 }]}</t>
+  </si>
+  <si>
+    <t>[{"ad":"&lt;html&gt;&lt;body&gt;&lt;script type=\"text\/javascript\"&gt;var ut_ju = 'http://stgads.undertone.com/aj';ut = new Object();ut.bidid='21b46f0d859b33';ut.bannerid=1196449;ut.zoneid=137770;ut.hbprice=4.00;ut.width=1;ut.height=1;ut.adaptor='prebid';ut.pid=3470;ut.extpid='10433394';ut.domain='ranker.com';&lt;\/script&gt;&lt;script type=\"text/javascript\" src=\"http://cdn.undertone.com/js/ajs.js\"&gt;&lt;\/script&gt;&lt;\/body&gt;&lt;\/html&gt;","publisherId": 3470,"bidRequestId": "21b46f0d859b33","placementId": "10433394","adId": 1196449,"campaignId": 297398,"height": 1,"width": 1,"currency": "USD","cpm": 4,"adaptor": "prebid","netRevenue": "true"}]</t>
+  </si>
+  <si>
+    <t>[{"ad":"&lt;html&gt;&lt;body&gt;&lt;script type=\"text\/javascript\"&gt;var ut_ju = 'http://stgads.undertone.com/aj';ut = new Object();ut.bidid='21b46f0d859b99';ut.bannerid=1179961;ut.zoneid=152010;ut.hbprice=7.00;ut.width=1;ut.height=1;ut.adaptor='prebid';ut.pid=3470;ut.extpid='10433394';ut.domain='ranker.com';&lt;\/script&gt;&lt;script type=\"text/javascript\" src=\"http://cdn.undertone.com/js/ajs.js\"&gt;&lt;\/script&gt;&lt;\/body&gt;&lt;\/html&gt;","publisherId": 3470,"bidRequestId": "21b46f0d859b99","placementId": "10433394","adId": 1179961,"campaignId": 292801,"height": 1,"width": 1,"currency": "USD","cpm": 7,"adaptor": "prebid","netRevenue": "true"}]</t>
+  </si>
+  <si>
+    <t>[{"ad":"&lt;html&gt;&lt;body&gt;&lt;script type=\"text\/javascript\"&gt;var ut_ju = 'http://stgads.undertone.com/aj';ut = new Object();ut.bidid='21b46f0d859b33';ut.bannerid=1196449;ut.zoneid=137770;ut.hbprice=4.00;ut.width=1;ut.height=1;ut.adaptor='prebid';ut.pid=3470;ut.extpid='';ut.domain='ranker.com';&lt;\/script&gt;&lt;script type=\"text/javascript\" src=\"http://cdn.undertone.com/js/ajs.js\"&gt;&lt;\/script&gt;&lt;\/body&gt;&lt;\/html&gt;","publisherId": 3470,"bidRequestId": "21b46f0d859b33","placementId": "","adId": 1196449,"campaignId": 297398,"height": 1,"width": 1,"currency": "USD","cpm": 4,"adaptor": "prebid","netRevenue": "true"}]</t>
+  </si>
+  <si>
+    <t>[{"ad":"&lt;html&gt;&lt;body&gt;&lt;script type=\"text\/javascript\"&gt;var ut_ju = 'http://stgads.undertone.com/aj';ut = new Object();ut.bidid='21b46f0d859b47';ut.bannerid=1196449;ut.zoneid=137770;ut.hbprice=4.00;ut.width=1;ut.height=1;ut.adaptor='prebid';ut.pid=3470;ut.extpid='10433394';ut.domain='ranker.com';&lt;\/script&gt;&lt;script type=\"text/javascript\" src=\"http://cdn.undertone.com/js/ajs.js\"&gt;&lt;\/script&gt;&lt;\/body&gt;&lt;\/html&gt;","publisherId": 3470,"bidRequestId": "21b46f0d859b47","placementId": "10433394","adId": 1196449,"campaignId": 297398,"height": 1,"width": 1,"currency": "USD","cpm": 4,"adaptor": "prebid","netRevenue": "true"}]</t>
   </si>
 </sst>
 </file>
@@ -986,8 +998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{605AD3CC-41F2-49AA-9F70-5058AA94EA10}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1357,7 +1369,7 @@
         <v>60</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>42</v>
+        <v>70</v>
       </c>
       <c r="G13" s="3">
         <v>0</v>
@@ -1413,7 +1425,7 @@
         <v>62</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>42</v>
+        <v>70</v>
       </c>
       <c r="G15" s="3">
         <v>0</v>
@@ -1442,7 +1454,7 @@
         <v>63</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="G16" s="3">
         <v>1</v>
@@ -1498,7 +1510,7 @@
         <v>64</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>44</v>
+        <v>72</v>
       </c>
       <c r="G18" s="3">
         <v>0</v>
@@ -1608,7 +1620,7 @@
         <v>68</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="G22" s="3">
         <v>0</v>

</xml_diff>